<commit_message>
solve error from New Contact test
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BDF281C4-E743-4952-9FD1-0A4FB63AEEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QA\Proejcts\MaveProject\POM Framwork\POMFramwork\src\main\java\com\crm\qa\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520A125-0DCD-4DA5-AB0B-5B9D2BCABB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{660EDF8C-1371-4A51-9654-D889AC974FDA}"/>
   </bookViews>
@@ -11,28 +16,16 @@
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>title</t>
   </si>
@@ -65,6 +58,24 @@
   </si>
   <si>
     <t>janvi</t>
+  </si>
+  <si>
+    <t>mox</t>
+  </si>
+  <si>
+    <t>bhikhabhai</t>
+  </si>
+  <si>
+    <t>patel</t>
+  </si>
+  <si>
+    <t>darji</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Tuxedo</t>
   </si>
 </sst>
 </file>
@@ -441,7 +452,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" activeCellId="1" sqref="C3 C18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,8 +499,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Test Added. - Task Page Test - Deals Page Test
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QA\Proejcts\MaveProject\POM Framwork\POMFramwork\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520A125-0DCD-4DA5-AB0B-5B9D2BCABB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4112E8C5-C99C-4A3B-89F0-5D590A6B8740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{660EDF8C-1371-4A51-9654-D889AC974FDA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{660EDF8C-1371-4A51-9654-D889AC974FDA}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="deals" sheetId="2" r:id="rId2"/>
+    <sheet name="Task" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>title</t>
   </si>
@@ -76,6 +78,51 @@
   </si>
   <si>
     <t>Tuxedo</t>
+  </si>
+  <si>
+    <t>Black Friday</t>
+  </si>
+  <si>
+    <t>Wight Monday</t>
+  </si>
+  <si>
+    <t>Thaks Giving</t>
+  </si>
+  <si>
+    <t>Canada Day</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>deal</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>Title1</t>
+  </si>
+  <si>
+    <t>Title2</t>
+  </si>
+  <si>
+    <t>Title3</t>
+  </si>
+  <si>
+    <t>Title4</t>
+  </si>
+  <si>
+    <t>Case1</t>
+  </si>
+  <si>
+    <t>Case2</t>
+  </si>
+  <si>
+    <t>Case3</t>
+  </si>
+  <si>
+    <t>Case4</t>
   </si>
 </sst>
 </file>
@@ -132,9 +179,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3524B09E-4DDB-4C5A-917A-47AAAE0E901F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -530,4 +578,148 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC9ADBB-7513-4E8F-A7AF-0483DEA5F15C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB29F1-F4FD-46AB-A5ED-BEE1E362FAB0}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>